<commit_message>
Updated chemical curation cleaning
</commit_message>
<xml_diff>
--- a/input/dictionaries/age_category_dict.xlsx
+++ b/input/dictionaries/age_category_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\CvT Database\input\dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FDB2F3-0507-4BA3-9865-CECB8FC300A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95600E8-EB22-4401-BEDC-0766CF71D533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="1440" windowWidth="17280" windowHeight="8964" xr2:uid="{B420EC6F-A2F6-4A7B-BBC7-24FB3BFDC94C}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="16635" windowHeight="8175" xr2:uid="{B420EC6F-A2F6-4A7B-BBC7-24FB3BFDC94C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>mouse</t>
   </si>
   <si>
-    <t>nonhuman primate</t>
-  </si>
-  <si>
     <t>rat</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>week</t>
+  </si>
+  <si>
+    <t>monkey</t>
   </si>
 </sst>
 </file>
@@ -436,38 +436,38 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -490,10 +490,10 @@
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -516,10 +516,10 @@
         <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -542,12 +542,12 @@
         <v>45</v>
       </c>
       <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -568,12 +568,12 @@
         <v>240</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1.25</v>
@@ -594,7 +594,7 @@
         <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>